<commit_message>
add new single user
</commit_message>
<xml_diff>
--- a/Data Files/New Employees Excel.xlsx
+++ b/Data Files/New Employees Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afaa1\Katalon Studio\PROJECT-WEB.git\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF1747C-7158-4AB7-BC0E-62444B1E8A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFC9F74-EF96-4D15-A5FB-099F303419F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">Sheet2!$A2</f>
-        <v>Chen132327</v>
+        <v>Chen125736</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">Sheet2!$A3</f>
-        <v>Ehi132327</v>
+        <v>Ehi125736</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -537,35 +537,35 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">B2&amp;C2</f>
-        <v>Chen132327</v>
+        <v>Chen125736</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">TEXT(D2,"hhmmss")</f>
-        <v>132327</v>
+        <v>125736</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">NOW()</f>
-        <v>44868.5579462963</v>
+        <v>44872.54000173611</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f ca="1">B3&amp;C3</f>
-        <v>Ehi132327</v>
+        <v>Ehi125736</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="str">
         <f ca="1">TEXT(D3,"hhmmss")</f>
-        <v>132327</v>
+        <v>125736</v>
       </c>
       <c r="D3" s="1">
         <f ca="1">NOW()</f>
-        <v>44868.5579462963</v>
+        <v>44872.54000173611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>